<commit_message>
upd theory of discrete math + rename comp system to CS and discrete math to DM
</commit_message>
<xml_diff>
--- a/1 semester/subjects.xlsx
+++ b/1 semester/subjects.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeloki\Documents\MAI\1 semester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19CDC2-A1F7-456F-9501-2F099906649B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3468" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3468" windowWidth="17280" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>иностранный язык</t>
   </si>
@@ -64,12 +63,18 @@
   </si>
   <si>
     <t>зачет</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>DM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,11 +385,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,6 +423,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -437,6 +445,9 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>